<commit_message>
Seção 5 - mesclar tabelas
</commit_message>
<xml_diff>
--- a/BaseCargos.xlsx
+++ b/BaseCargos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnny\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJETOS\UDEMY\Power_BI_Completo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -255,7 +255,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -293,7 +293,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -365,7 +365,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -518,10 +518,14 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H26"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>